<commit_message>
Update IP - EX 12 - Funcao SE II (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 12 - Funcao SE II (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 12 - Funcao SE II (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B3A2268-E162-431D-88D0-1D3B61ACEC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E05134-5BFF-46F3-961A-AA385260D7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>OUTRAS INFORMAÇÕES</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>VALOR VENDIDO</t>
+  </si>
+  <si>
+    <t>produto</t>
   </si>
 </sst>
 </file>
@@ -911,7 +914,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1076,6 +1079,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Moeda" xfId="4" builtinId="4"/>
@@ -1614,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1793,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q96"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16:Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,7 +2017,9 @@
       <c r="M13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="N13" s="60"/>
+      <c r="N13" s="60" t="s">
+        <v>37</v>
+      </c>
       <c r="O13" s="61"/>
       <c r="P13" s="62"/>
     </row>
@@ -2065,9 +2071,16 @@
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="18">
-        <v>89</v>
-      </c>
-      <c r="K16" s="63"/>
+        <v>100</v>
+      </c>
+      <c r="K16" s="63">
+        <f>IF(NOT(ISERR(FIND(LOWER("som"),LOWER(N13)))),B18,
+IF(OR(NOT(ISERR(FIND(LOWER("média"),LOWER(N13)))),NOT(ISERR(FIND(LOWER("media"),LOWER(N13))))),D18,
+IF(NOT(ISERR(FIND(LOWER("cont"),LOWER(N13)))),F18,
+IF(NOT(ISERR(FIND(LOWER("prod"),LOWER(N13)))),H18,
+"Operação não encontrada"))))</f>
+        <v>248400000</v>
+      </c>
       <c r="L16" s="64"/>
       <c r="M16" s="64"/>
       <c r="N16" s="64"/>
@@ -2100,10 +2113,22 @@
       <c r="Q17" s="68"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="B18" s="19">
+        <f>SUM(B12:B17)</f>
+        <v>199</v>
+      </c>
+      <c r="D18" s="72">
+        <f>AVERAGE(D12:D17)</f>
+        <v>33.166666666666664</v>
+      </c>
+      <c r="F18" s="19">
+        <f>COUNTA(F12:F17)</f>
+        <v>6</v>
+      </c>
+      <c r="H18" s="19">
+        <f>PRODUCT(H12:H17)</f>
+        <v>248400000</v>
+      </c>
       <c r="K18" s="66"/>
       <c r="L18" s="67"/>
       <c r="M18" s="67"/>
@@ -2369,7 +2394,7 @@
   <dimension ref="B1:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>